<commit_message>
Update Project 3 Questions and p3-results with latest findings
</commit_message>
<xml_diff>
--- a/Project 3/p3-results.xlsx
+++ b/Project 3/p3-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec6cd1f718787101/Documents/Quinnipiac/Spring-2025/CSC350/Project 3/Project-3---Clustering/Project 3/java/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milenamartinon/Desktop/SPRING 25/CSC 350/Project 3/Project 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{6D7F0FA9-3B6F-4247-966F-E9988896F06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB9BF9FE-13EA-482A-AC84-FA138694F4ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E394CB-7560-F341-BB6A-7BBD7AAB1B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{FF08A997-3A99-4B2C-BEDC-14A11E32874A}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{FF08A997-3A99-4B2C-BEDC-14A11E32874A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Data File</t>
   </si>
@@ -156,13 +156,19 @@
   </si>
   <si>
     <t>EXERCISE 3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +180,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -215,6 +228,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,23 +547,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3C8089-43CC-4DB7-89C7-70525ACCD8EA}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="2" customWidth="1"/>
-    <col min="5" max="7" width="8.73046875" style="2"/>
-    <col min="8" max="8" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="8.73046875" style="2"/>
+    <col min="2" max="3" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="2"/>
+    <col min="6" max="6" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="2"/>
+    <col min="8" max="8" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="2"/>
+    <col min="10" max="17" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
@@ -569,7 +588,7 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,7 +635,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -637,8 +656,35 @@
         <f>MIN(B3:D3)</f>
         <v>22.5430817312639</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H3" s="4">
+        <v>22.541966326743701</v>
+      </c>
+      <c r="J3" s="2">
+        <v>22.429426987332899</v>
+      </c>
+      <c r="K3" s="2">
+        <v>22.3846201831707</v>
+      </c>
+      <c r="L3" s="2">
+        <v>22.638872942387099</v>
+      </c>
+      <c r="M3" s="2">
+        <v>22.429426987332899</v>
+      </c>
+      <c r="N3" s="2">
+        <v>22.641297160130001</v>
+      </c>
+      <c r="O3" s="2">
+        <v>22.429426987332899</v>
+      </c>
+      <c r="P3" s="2">
+        <v>22.3846201831707</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>22.4283245797067</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -659,8 +705,38 @@
         <f t="shared" ref="F4:F24" si="1">MIN(B4:D4)</f>
         <v>9.7972494149063394</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H4" s="4">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="J4" s="2">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="K4" s="2">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="L4" s="2">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="M4" s="2">
+        <v>9.7981551468909593</v>
+      </c>
+      <c r="N4" s="2">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="O4" s="2">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="P4" s="2">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>9.7972494149063394</v>
+      </c>
+      <c r="R4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -681,8 +757,38 @@
         <f t="shared" si="1"/>
         <v>1.12140865001139</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H5" s="4">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1.12140865001139</v>
+      </c>
+      <c r="R5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -703,8 +809,35 @@
         <f t="shared" si="1"/>
         <v>0.50613459342410205</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H6" s="4">
+        <v>0.33638761656947502</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.33638761656947502</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.345569198312149</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.345569198312149</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.345569198312149</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.33638761656947502</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.36904471329701399</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.345569198312149</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.33704147201486401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -725,8 +858,38 @@
         <f t="shared" si="1"/>
         <v>0.55971682890649099</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H7" s="4">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0.55971682890649099</v>
+      </c>
+      <c r="R7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -747,8 +910,38 @@
         <f t="shared" si="1"/>
         <v>0.51026753969379501</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H8" s="4">
+        <v>6.69496542660006</v>
+      </c>
+      <c r="J8" s="2">
+        <v>6.8417570676701596</v>
+      </c>
+      <c r="K8" s="2">
+        <v>6.69496542660006</v>
+      </c>
+      <c r="L8" s="2">
+        <v>6.3843814412801896</v>
+      </c>
+      <c r="M8" s="2">
+        <v>6.8417570676701596</v>
+      </c>
+      <c r="N8" s="2">
+        <v>6.69496542660006</v>
+      </c>
+      <c r="O8" s="2">
+        <v>6.8417570676701596</v>
+      </c>
+      <c r="P8" s="2">
+        <v>6.8417570676701596</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>6.3843814412801896</v>
+      </c>
+      <c r="R8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -769,8 +962,38 @@
         <f t="shared" si="1"/>
         <v>0.47006206486089502</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H9" s="4">
+        <v>9.0426940999840308</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9.0426940999840308</v>
+      </c>
+      <c r="K9" s="2">
+        <v>9.7293938006062994</v>
+      </c>
+      <c r="L9" s="2">
+        <v>9.7293938006062994</v>
+      </c>
+      <c r="M9" s="2">
+        <v>18.2976766853043</v>
+      </c>
+      <c r="N9" s="2">
+        <v>9.0426940999840308</v>
+      </c>
+      <c r="O9" s="2">
+        <v>9.7293938006062994</v>
+      </c>
+      <c r="P9" s="2">
+        <v>9.7293938006062994</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>9.0426940999840308</v>
+      </c>
+      <c r="R9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -791,8 +1014,35 @@
         <f t="shared" si="1"/>
         <v>0.51057188242228402</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H10" s="4">
+        <v>8.70883502813383</v>
+      </c>
+      <c r="J10" s="2">
+        <v>9.0694649952438393</v>
+      </c>
+      <c r="K10" s="2">
+        <v>10.577553829768499</v>
+      </c>
+      <c r="L10" s="2">
+        <v>8.70883502813383</v>
+      </c>
+      <c r="M10" s="2">
+        <v>10.578650337052</v>
+      </c>
+      <c r="N10" s="2">
+        <v>8.7088092889942992</v>
+      </c>
+      <c r="O10" s="2">
+        <v>8.70883502813383</v>
+      </c>
+      <c r="P10" s="2">
+        <v>9.1103212675399501</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>9.0694649952438393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -813,8 +1063,38 @@
         <f t="shared" si="1"/>
         <v>0.463040616666479</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H11" s="4">
+        <v>6.8998146794585802</v>
+      </c>
+      <c r="J11" s="2">
+        <v>7.3319909444984699</v>
+      </c>
+      <c r="K11" s="2">
+        <v>6.8479746403691104</v>
+      </c>
+      <c r="L11" s="2">
+        <v>6.8998146794585802</v>
+      </c>
+      <c r="M11" s="2">
+        <v>7.3319909444984699</v>
+      </c>
+      <c r="N11" s="2">
+        <v>6.8998146794585802</v>
+      </c>
+      <c r="O11" s="2">
+        <v>6.8998146794585802</v>
+      </c>
+      <c r="P11" s="2">
+        <v>6.8479746403691104</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>7.3319909444984699</v>
+      </c>
+      <c r="R11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -835,8 +1115,35 @@
         <f t="shared" si="1"/>
         <v>0.45367484826115601</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H12" s="4">
+        <v>6.0671907663239697</v>
+      </c>
+      <c r="J12" s="2">
+        <v>6.3802043727122602</v>
+      </c>
+      <c r="K12" s="2">
+        <v>6.3802043727122602</v>
+      </c>
+      <c r="L12" s="2">
+        <v>6.3735141686971799</v>
+      </c>
+      <c r="M12" s="2">
+        <v>6.0671907663239697</v>
+      </c>
+      <c r="N12" s="2">
+        <v>6.3802043727122602</v>
+      </c>
+      <c r="O12" s="2">
+        <v>10.5265348463649</v>
+      </c>
+      <c r="P12" s="2">
+        <v>6.0671907663239697</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>6.8869665858309697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -857,8 +1164,35 @@
         <f t="shared" si="1"/>
         <v>0.35259721941288202</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H13" s="4">
+        <v>6.1905284490298103</v>
+      </c>
+      <c r="J13" s="2">
+        <v>6.1905284490298103</v>
+      </c>
+      <c r="K13" s="2">
+        <v>6.1905284490298103</v>
+      </c>
+      <c r="L13" s="2">
+        <v>6.7161736385278097</v>
+      </c>
+      <c r="M13" s="2">
+        <v>6.1766118569259802</v>
+      </c>
+      <c r="N13" s="2">
+        <v>6.1766118569259802</v>
+      </c>
+      <c r="O13" s="2">
+        <v>6.1905284490298103</v>
+      </c>
+      <c r="P13" s="2">
+        <v>6.1905284490298103</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>6.1808571887563399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -879,8 +1213,35 @@
         <f t="shared" si="1"/>
         <v>0.41331275915580801</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H14" s="4">
+        <v>7.6038071444614399</v>
+      </c>
+      <c r="J14" s="2">
+        <v>7.5474563295486101</v>
+      </c>
+      <c r="K14" s="2">
+        <v>7.6761816308303796</v>
+      </c>
+      <c r="L14" s="2">
+        <v>7.5652344489831904</v>
+      </c>
+      <c r="M14" s="2">
+        <v>8.0025282382155503</v>
+      </c>
+      <c r="N14" s="2">
+        <v>7.5379780855500904</v>
+      </c>
+      <c r="O14" s="2">
+        <v>7.52074384239359</v>
+      </c>
+      <c r="P14" s="2">
+        <v>7.5597768681289299</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>7.6038071444614399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -901,8 +1262,35 @@
         <f t="shared" si="1"/>
         <v>0.46102009633985802</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="H15" s="4">
+        <v>0.29195881139122198</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.29052642476740298</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.28947602411886503</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.29195881139122198</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.29198208906158901</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.29398060498425099</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.30230228130627501</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0.31508403032235799</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0.29402813796384702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -923,8 +1311,38 @@
         <f t="shared" si="1"/>
         <v>0.54217027264039896</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H16" s="4">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0.54217027264039896</v>
+      </c>
+      <c r="R16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -945,8 +1363,35 @@
         <f t="shared" si="1"/>
         <v>0.42010081663958099</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H17" s="4">
+        <v>0.73854470165158903</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.73854470165158903</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.73854470165158903</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.73483909231449596</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.73483909231449596</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.73854470165158903</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.73854470165158903</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.73854470165158903</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0.73854470165158903</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -967,8 +1412,35 @@
         <f t="shared" si="1"/>
         <v>0.39274524877113198</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H18" s="4">
+        <v>1.4832748222186301</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2.1223069289018701</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.4832748222186301</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1.4832748222186301</v>
+      </c>
+      <c r="M18" s="2">
+        <v>2.1223069289018701</v>
+      </c>
+      <c r="N18" s="2">
+        <v>2.1223069289018701</v>
+      </c>
+      <c r="O18" s="2">
+        <v>1.4832748222186301</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1.4832748222186301</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>1.4832748222186301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -989,8 +1461,35 @@
         <f t="shared" si="1"/>
         <v>0.43096019615699499</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H19" s="4">
+        <v>1.5652926334756601</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.56594670734242</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.5652926334756601</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1.5652926334756601</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1.56594670734242</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1.5652926334756601</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1.5652926334756601</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1.5652926334756601</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>1.56470230382949</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1011,8 +1510,35 @@
         <f t="shared" si="1"/>
         <v>0.43472164015984599</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H20" s="4">
+        <v>3.1803719036714102</v>
+      </c>
+      <c r="J20" s="2">
+        <v>3.1803719036714102</v>
+      </c>
+      <c r="K20" s="2">
+        <v>4.03361824086823</v>
+      </c>
+      <c r="L20" s="2">
+        <v>3.3853840538239499</v>
+      </c>
+      <c r="M20" s="2">
+        <v>3.1803719036714102</v>
+      </c>
+      <c r="N20" s="2">
+        <v>3.3853840538239499</v>
+      </c>
+      <c r="O20" s="2">
+        <v>3.1803719036714102</v>
+      </c>
+      <c r="P20" s="2">
+        <v>3.3853840538239499</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>3.1803719036714102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1033,8 +1559,38 @@
         <f t="shared" si="1"/>
         <v>0.38952330303014798</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H21" s="4">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="O21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1.68893109303075</v>
+      </c>
+      <c r="R21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1055,8 +1611,35 @@
         <f t="shared" si="1"/>
         <v>0.368137089347714</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H22" s="4">
+        <v>2.3116449243396202</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2.3116449243396202</v>
+      </c>
+      <c r="K22" s="2">
+        <v>2.3116449243396202</v>
+      </c>
+      <c r="L22" s="2">
+        <v>2.3116449243396202</v>
+      </c>
+      <c r="M22" s="2">
+        <v>2.3116449243396202</v>
+      </c>
+      <c r="N22" s="2">
+        <v>2.3116449243396202</v>
+      </c>
+      <c r="O22" s="2">
+        <v>3.7296710262705699</v>
+      </c>
+      <c r="P22" s="2">
+        <v>2.3116449243396202</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>2.3116449239999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1077,8 +1660,35 @@
         <f t="shared" si="1"/>
         <v>0.39206627794288901</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H23" s="4">
+        <v>2.1208650192724199</v>
+      </c>
+      <c r="J23" s="2">
+        <v>2.1208650192724199</v>
+      </c>
+      <c r="K23" s="2">
+        <v>2.1208650192724199</v>
+      </c>
+      <c r="L23" s="2">
+        <v>2.1208650192724199</v>
+      </c>
+      <c r="M23" s="2">
+        <v>2.1208650192724199</v>
+      </c>
+      <c r="N23" s="2">
+        <v>2.1208650192724199</v>
+      </c>
+      <c r="O23" s="2">
+        <v>5.9180577874489098</v>
+      </c>
+      <c r="P23" s="2">
+        <v>2.1208650192724199</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>2.1208650192724199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1098,6 +1708,36 @@
       <c r="F24" s="2">
         <f t="shared" si="1"/>
         <v>1.25831324316183</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="P24" s="2">
+        <v>3.5987869723542998</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>1.25831324316183</v>
+      </c>
+      <c r="R24" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>